<commit_message>
First machine test. Updated some experimental settings and some imaging functionalities
</commit_message>
<xml_diff>
--- a/.config/acquisitionConfig/roi.csv.xlsx
+++ b/.config/acquisitionConfig/roi.csv.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,12 +10,12 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6007B0-0ECB-4190-943A-A23D44CEBA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Angle</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>EvapDOdt3</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>SideOdtCamera</t>
   </si>
 </sst>
 </file>
@@ -109,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -117,12 +123,14 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,25 +411,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="5" width="5.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="true"/>
+    <col min="2" max="2" width="5.140625" customWidth="true"/>
+    <col min="3" max="3" width="5.140625" customWidth="true"/>
+    <col min="6" max="6" width="11.140625" customWidth="true"/>
+    <col min="7" max="7" width="11.28515625" customWidth="true"/>
+    <col min="8" max="8" width="6.28515625" customWidth="true"/>
+    <col min="9" max="9" width="2.85546875" customWidth="true"/>
+    <col min="10" max="10" width="10.5703125" customWidth="true"/>
+    <col min="4" max="4" width="5.140625" customWidth="true"/>
+    <col min="5" max="5" width="5.140625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -447,7 +457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -473,7 +483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -499,7 +509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -525,33 +535,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>1150</v>
-      </c>
-      <c r="C5">
-        <v>1350</v>
-      </c>
-      <c r="D5">
-        <v>1700</v>
-      </c>
-      <c r="E5">
-        <v>1900</v>
-      </c>
-      <c r="F5">
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="0">
+        <v>1159</v>
+      </c>
+      <c r="C5" s="0">
+        <v>1319</v>
+      </c>
+      <c r="D5" s="0">
+        <v>1668</v>
+      </c>
+      <c r="E5" s="0">
+        <v>1848</v>
+      </c>
+      <c r="F5" s="0">
         <v>2160</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>2560</v>
       </c>
-      <c r="H5">
-        <v>-9.1999999999999993</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="H5" s="0">
+        <v>350.80000000000001</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -577,7 +587,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -601,6 +611,32 @@
       </c>
       <c r="H7">
         <v>-10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0">
+        <v>301</v>
+      </c>
+      <c r="C8" s="0">
+        <v>645</v>
+      </c>
+      <c r="D8" s="0">
+        <v>654</v>
+      </c>
+      <c r="E8" s="0">
+        <v>1018</v>
+      </c>
+      <c r="F8" s="0">
+        <v>1080</v>
+      </c>
+      <c r="G8" s="0">
+        <v>1920</v>
+      </c>
+      <c r="H8" s="0">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fixing for centerfit
</commit_message>
<xml_diff>
--- a/.config/acquisitionConfig/roi.csv.xlsx
+++ b/.config/acquisitionConfig/roi.csv.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Angle</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>SideOdtCamera</t>
+  </si>
+  <si>
+    <t>Bec</t>
   </si>
 </sst>
 </file>
@@ -537,19 +540,19 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0">
-        <v>1159</v>
+        <v>1111</v>
       </c>
       <c r="C5" s="0">
-        <v>1319</v>
+        <v>1329</v>
       </c>
       <c r="D5" s="0">
-        <v>1668</v>
+        <v>1630</v>
       </c>
       <c r="E5" s="0">
-        <v>1848</v>
+        <v>1882</v>
       </c>
       <c r="F5" s="0">
         <v>2160</v>

</xml_diff>

<commit_message>
changed some ROI parameters
</commit_message>
<xml_diff>
--- a/.config/acquisitionConfig/roi.csv.xlsx
+++ b/.config/acquisitionConfig/roi.csv.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Angle</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>SideOdtCamera</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>NiLattice</t>
+  </si>
+  <si>
+    <t>Bec</t>
   </si>
   <si>
     <t>Bec</t>
@@ -414,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
@@ -540,19 +549,19 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0">
-        <v>1111</v>
+        <v>1172</v>
       </c>
       <c r="C5" s="0">
-        <v>1329</v>
+        <v>1350</v>
       </c>
       <c r="D5" s="0">
-        <v>1630</v>
+        <v>1667</v>
       </c>
       <c r="E5" s="0">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="F5" s="0">
         <v>2160</v>
@@ -561,7 +570,7 @@
         <v>2560</v>
       </c>
       <c r="H5" s="0">
-        <v>350.80000000000001</v>
+        <v>349.10000000000002</v>
       </c>
     </row>
     <row r="6">
@@ -640,6 +649,32 @@
       </c>
       <c r="H8" s="0">
         <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="0">
+        <v>1107</v>
+      </c>
+      <c r="C9" s="0">
+        <v>1417</v>
+      </c>
+      <c r="D9" s="0">
+        <v>1740</v>
+      </c>
+      <c r="E9" s="0">
+        <v>1814</v>
+      </c>
+      <c r="F9" s="0">
+        <v>2160</v>
+      </c>
+      <c r="G9" s="0">
+        <v>2560</v>
+      </c>
+      <c r="H9" s="0">
+        <v>349.10000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the mask bug. Added sub-ROI functions
</commit_message>
<xml_diff>
--- a/.config/acquisitionConfig/roi.csv.xlsx
+++ b/.config/acquisitionConfig/roi.csv.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Work\MuscleMuseum\.config\acquisitionConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6007B0-0ECB-4190-943A-A23D44CEBA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF4AA8C-DE48-4888-9771-0A739CE92B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,81 +25,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Angle</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>X1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ImageSizeY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ImageSizeX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EvapDOdt1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EvapDOdt2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EvapDOdt3</t>
+  </si>
+  <si>
+    <t>SideOdtCamera</t>
+  </si>
+  <si>
     <t>Bec</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ImageSizeY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ImageSizeX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EvapDOdt1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EvapDOdt2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>testRoi</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TestTest</t>
-  </si>
-  <si>
-    <t>EvapDOdt3</t>
-  </si>
-  <si>
-    <t>Bec</t>
-  </si>
-  <si>
-    <t>SideOdtCamera</t>
-  </si>
-  <si>
-    <t>Bec</t>
   </si>
   <si>
     <t>NiLattice</t>
   </si>
   <si>
-    <t>Bec</t>
-  </si>
-  <si>
-    <t>Bec</t>
-  </si>
-  <si>
-    <t>NiLattice</t>
+    <t>SubRoiCenterSize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubRoiNRowColumn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubRoiSeparation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -130,7 +133,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -138,14 +141,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,55 +427,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="true"/>
-    <col min="2" max="2" width="5.140625" customWidth="true"/>
-    <col min="3" max="3" width="5.140625" customWidth="true"/>
-    <col min="6" max="6" width="11.140625" customWidth="true"/>
-    <col min="7" max="7" width="11.28515625" customWidth="true"/>
-    <col min="8" max="8" width="6.28515625" customWidth="true"/>
-    <col min="9" max="9" width="2.85546875" customWidth="true"/>
-    <col min="10" max="10" width="10.5703125" customWidth="true"/>
-    <col min="4" max="4" width="5.140625" customWidth="true"/>
-    <col min="5" max="5" width="5.140625" customWidth="true"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="5" width="5.140625" customWidth="1"/>
+    <col min="6" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="3.140625" customWidth="1"/>
+    <col min="13" max="14" width="2.140625" customWidth="1"/>
+    <col min="15" max="16" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
       </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>300</v>
@@ -497,10 +507,16 @@
       <c r="H2">
         <v>0</v>
       </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>550</v>
@@ -523,10 +539,16 @@
       <c r="H3">
         <v>0</v>
       </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>750</v>
@@ -549,74 +571,92 @@
       <c r="H4">
         <v>0</v>
       </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>1172</v>
+      </c>
+      <c r="C5">
+        <v>1350</v>
+      </c>
+      <c r="D5">
+        <v>1667</v>
+      </c>
+      <c r="E5">
+        <v>1881</v>
+      </c>
+      <c r="F5">
+        <v>2160</v>
+      </c>
+      <c r="G5">
+        <v>2560</v>
+      </c>
+      <c r="H5">
+        <v>349.1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="0">
-        <v>1172</v>
-      </c>
-      <c r="C5" s="0">
-        <v>1350</v>
-      </c>
-      <c r="D5" s="0">
-        <v>1667</v>
-      </c>
-      <c r="E5" s="0">
-        <v>1881</v>
-      </c>
-      <c r="F5" s="0">
-        <v>2160</v>
-      </c>
-      <c r="G5" s="0">
-        <v>2560</v>
-      </c>
-      <c r="H5" s="0">
-        <v>349.10000000000002</v>
-      </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>301</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>645</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>654</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>1018</v>
       </c>
       <c r="F6">
-        <v>100</v>
+        <v>1080</v>
       </c>
       <c r="G6">
-        <v>200</v>
+        <v>1920</v>
       </c>
       <c r="H6">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7">
-        <v>1150</v>
+        <v>1060</v>
       </c>
       <c r="C7">
-        <v>1350</v>
+        <v>1466</v>
       </c>
       <c r="D7">
-        <v>1000</v>
+        <v>1733</v>
       </c>
       <c r="E7">
-        <v>1900</v>
+        <v>1813</v>
       </c>
       <c r="F7">
         <v>2160</v>
@@ -625,59 +665,13 @@
         <v>2560</v>
       </c>
       <c r="H7">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="0">
-        <v>301</v>
-      </c>
-      <c r="C8" s="0">
-        <v>645</v>
-      </c>
-      <c r="D8" s="0">
-        <v>654</v>
-      </c>
-      <c r="E8" s="0">
-        <v>1018</v>
-      </c>
-      <c r="F8" s="0">
-        <v>1080</v>
-      </c>
-      <c r="G8" s="0">
-        <v>1920</v>
-      </c>
-      <c r="H8" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="0">
-        <v>1060</v>
-      </c>
-      <c r="C9" s="0">
-        <v>1466</v>
-      </c>
-      <c r="D9" s="0">
-        <v>1733</v>
-      </c>
-      <c r="E9" s="0">
-        <v>1813</v>
-      </c>
-      <c r="F9" s="0">
-        <v>2160</v>
-      </c>
-      <c r="G9" s="0">
-        <v>2560</v>
-      </c>
-      <c r="H9" s="0">
-        <v>349.10000000000002</v>
+        <v>349.1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some changes during exp run
</commit_message>
<xml_diff>
--- a/.config/acquisitionConfig/roi.csv.xlsx
+++ b/.config/acquisitionConfig/roi.csv.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Work\MuscleMuseum\.config\acquisitionConfig\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\_Li\Machine Code\MuscleMuseum\.config\acquisitionConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF4AA8C-DE48-4888-9771-0A739CE92B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00025E33-BF68-4E5E-AF5B-1661FA745351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Angle</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -103,6 +103,18 @@
   <si>
     <t>[100 100]</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NILatticeKd</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
   </si>
 </sst>
 </file>
@@ -427,21 +439,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="5" width="5.140625" customWidth="1"/>
-    <col min="6" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
     <col min="12" max="12" width="3.140625" customWidth="1"/>
     <col min="13" max="14" width="2.140625" customWidth="1"/>
     <col min="15" max="16" width="4.140625" customWidth="1"/>
@@ -674,6 +687,41 @@
         <v>19</v>
       </c>
     </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>820</v>
+      </c>
+      <c r="C8">
+        <v>1702</v>
+      </c>
+      <c r="D8">
+        <v>1707</v>
+      </c>
+      <c r="E8">
+        <v>1819</v>
+      </c>
+      <c r="F8">
+        <v>2160</v>
+      </c>
+      <c r="G8">
+        <v>2560</v>
+      </c>
+      <c r="H8">
+        <v>349.1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
start to work on BecBrowser
</commit_message>
<xml_diff>
--- a/.config/acquisitionConfig/roi.csv.xlsx
+++ b/.config/acquisitionConfig/roi.csv.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>Angle</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -193,6 +193,18 @@
   </si>
   <si>
     <t>[983 1560 30 100;1167 1596 100 100;806 1526 100 100;923 1549 50 100;1031 1569 40 100]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeMagicAi</t>
+  </si>
+  <si>
+    <t>[897 1572 100 50;995 1591 100 50;1142 1619 150 50]</t>
   </si>
   <si>
     <t>[1 1]</t>
@@ -525,7 +537,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -919,6 +931,41 @@
         <v>52</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="0">
+        <v>1016</v>
+      </c>
+      <c r="C12" s="0">
+        <v>1534</v>
+      </c>
+      <c r="D12" s="0">
+        <v>1755</v>
+      </c>
+      <c r="E12" s="0">
+        <v>1811</v>
+      </c>
+      <c r="F12" s="0">
+        <v>2160</v>
+      </c>
+      <c r="G12" s="0">
+        <v>2560</v>
+      </c>
+      <c r="H12" s="0">
+        <v>349.10000000000002</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implemented Triangle Wave fit
</commit_message>
<xml_diff>
--- a/.config/acquisitionConfig/roi.csv.xlsx
+++ b/.config/acquisitionConfig/roi.csv.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="81">
   <si>
     <t>Angle</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -205,6 +205,78 @@
   </si>
   <si>
     <t>[897 1572 100 50;995 1591 100 50;1142 1619 150 50]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>BMPDloop</t>
+  </si>
+  <si>
+    <t>[1064 1611 200 40]</t>
+  </si>
+  <si>
+    <t>[2 1]</t>
+  </si>
+  <si>
+    <t>[200 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalib</t>
+  </si>
+  <si>
+    <t>[975 1588 50 50]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[130 100]</t>
+  </si>
+  <si>
+    <t>BMPDloopTof3000</t>
+  </si>
+  <si>
+    <t>[1015 1602 260 50]</t>
+  </si>
+  <si>
+    <t>[2 1]</t>
+  </si>
+  <si>
+    <t>[340 100]</t>
+  </si>
+  <si>
+    <t>PdBoBm</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>PDBO</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>PDBO</t>
+  </si>
+  <si>
+    <t>[]</t>
   </si>
   <si>
     <t>[1 1]</t>
@@ -537,7 +609,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -966,6 +1038,181 @@
         <v>56</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="0">
+        <v>974</v>
+      </c>
+      <c r="C13" s="0">
+        <v>1554</v>
+      </c>
+      <c r="D13" s="0">
+        <v>1754</v>
+      </c>
+      <c r="E13" s="0">
+        <v>1830</v>
+      </c>
+      <c r="F13" s="0">
+        <v>2160</v>
+      </c>
+      <c r="G13" s="0">
+        <v>2560</v>
+      </c>
+      <c r="H13" s="0">
+        <v>349.10000000000002</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="0">
+        <v>1035</v>
+      </c>
+      <c r="C14" s="0">
+        <v>1491</v>
+      </c>
+      <c r="D14" s="0">
+        <v>1708</v>
+      </c>
+      <c r="E14" s="0">
+        <v>1838</v>
+      </c>
+      <c r="F14" s="0">
+        <v>2160</v>
+      </c>
+      <c r="G14" s="0">
+        <v>2560</v>
+      </c>
+      <c r="H14" s="0">
+        <v>349.10000000000002</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="0">
+        <v>924</v>
+      </c>
+      <c r="C15" s="0">
+        <v>1604</v>
+      </c>
+      <c r="D15" s="0">
+        <v>1704</v>
+      </c>
+      <c r="E15" s="0">
+        <v>1880</v>
+      </c>
+      <c r="F15" s="0">
+        <v>2160</v>
+      </c>
+      <c r="G15" s="0">
+        <v>2560</v>
+      </c>
+      <c r="H15" s="0">
+        <v>349.10000000000002</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="0">
+        <v>994</v>
+      </c>
+      <c r="C16" s="0">
+        <v>1588</v>
+      </c>
+      <c r="D16" s="0">
+        <v>1746</v>
+      </c>
+      <c r="E16" s="0">
+        <v>1822</v>
+      </c>
+      <c r="F16" s="0">
+        <v>2160</v>
+      </c>
+      <c r="G16" s="0">
+        <v>2560</v>
+      </c>
+      <c r="H16" s="0">
+        <v>349.10000000000002</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="0">
+        <v>1172</v>
+      </c>
+      <c r="C17" s="0">
+        <v>1332</v>
+      </c>
+      <c r="D17" s="0">
+        <v>1781</v>
+      </c>
+      <c r="E17" s="0">
+        <v>1819</v>
+      </c>
+      <c r="F17" s="0">
+        <v>2160</v>
+      </c>
+      <c r="G17" s="0">
+        <v>2560</v>
+      </c>
+      <c r="H17" s="0">
+        <v>349.10000000000002</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bug fixing. parameter updating
</commit_message>
<xml_diff>
--- a/.config/acquisitionConfig/roi.csv.xlsx
+++ b/.config/acquisitionConfig/roi.csv.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="101">
   <si>
     <t>Angle</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -319,6 +319,30 @@
   </si>
   <si>
     <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalib</t>
+  </si>
+  <si>
+    <t>[989 1570 50 50]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[130 100]</t>
+  </si>
+  <si>
+    <t>BMPDloopTof3000</t>
+  </si>
+  <si>
+    <t>[1019 1582 260 50]</t>
+  </si>
+  <si>
+    <t>[2 1]</t>
+  </si>
+  <si>
+    <t>[340 100]</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1135,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="B14" s="0">
         <v>1035</v>
@@ -1135,18 +1159,18 @@
         <v>349.10000000000002</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="B15" s="0">
         <v>924</v>
@@ -1170,13 +1194,13 @@
         <v>349.10000000000002</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
onsite changes including the selection of whether to representaveraged data
</commit_message>
<xml_diff>
--- a/.config/acquisitionConfig/roi.csv.xlsx
+++ b/.config/acquisitionConfig/roi.csv.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="457">
   <si>
     <t>Angle</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -655,6 +655,762 @@
   </si>
   <si>
     <t>[100 100]</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>EvapDOdt1</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLattice</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalib</t>
+  </si>
+  <si>
+    <t>[1132 981 100 50]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[130 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalib</t>
+  </si>
+  <si>
+    <t>[1132 981 100 50]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[130 100]</t>
+  </si>
+  <si>
+    <t>NILatticeKd</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalib</t>
+  </si>
+  <si>
+    <t>[1132 981 100 100]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[130 100]</t>
+  </si>
+  <si>
+    <t>NILatticeKd</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalib</t>
+  </si>
+  <si>
+    <t>[1091 939 100 100]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[130 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeBoBm</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLattice</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalib</t>
+  </si>
+  <si>
+    <t>[1093 837 100 100]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[130 100]</t>
+  </si>
+  <si>
+    <t>EvapDOdt1</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>EvapDOdt1</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalib</t>
+  </si>
+  <si>
+    <t>[1209 1239 100 100]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[130 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalib</t>
+  </si>
+  <si>
+    <t>[1200 1242 100 100]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[130 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeBoBm</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>EvapDOdt1</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NILatticeKd</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalib</t>
+  </si>
+  <si>
+    <t>[937 1344 100 100]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[130 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalib</t>
+  </si>
+  <si>
+    <t>[937 1344 100 100]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[130 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalib</t>
+  </si>
+  <si>
+    <t>[937 1344 100 100]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[170 100]</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>EvapDOdt1</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLattice</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLattice</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLattice</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLattice</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>EvapDOdt1</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLattice</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NILatticeKd</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalib</t>
+  </si>
+  <si>
+    <t>[937 1344 100 100]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[170 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalib</t>
+  </si>
+  <si>
+    <t>[1000 1357 100 100]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[170 100]</t>
+  </si>
+  <si>
+    <t>NiLattice</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NILatticeKd</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NILatticeKd</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeBoBm</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalib</t>
+  </si>
+  <si>
+    <t>[998 1357 130 100]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[170 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeBoBm</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>BMPDloopTof3000</t>
+  </si>
+  <si>
+    <t>[857 1387 260 50]</t>
+  </si>
+  <si>
+    <t>[2 1]</t>
+  </si>
+  <si>
+    <t>[560 100]</t>
+  </si>
+  <si>
+    <t>BMPDloopTof3000</t>
+  </si>
+  <si>
+    <t>[857 1387 260 75]</t>
+  </si>
+  <si>
+    <t>[2 1]</t>
+  </si>
+  <si>
+    <t>[560 100]</t>
+  </si>
+  <si>
+    <t>BMPDloopTof5000</t>
+  </si>
+  <si>
+    <t>[872 1418 260 75]</t>
+  </si>
+  <si>
+    <t>[2 1]</t>
+  </si>
+  <si>
+    <t>[560 100]</t>
+  </si>
+  <si>
+    <t>BMPDloopTof5000</t>
+  </si>
+  <si>
+    <t>[892 1417 170 85]</t>
+  </si>
+  <si>
+    <t>[2 1]</t>
+  </si>
+  <si>
+    <t>[700 100]</t>
+  </si>
+  <si>
+    <t>BMPDloopTof5000</t>
+  </si>
+  <si>
+    <t>[891 1407 170 85]</t>
+  </si>
+  <si>
+    <t>[2 1]</t>
+  </si>
+  <si>
+    <t>[700 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalibTof6000</t>
+  </si>
+  <si>
+    <t>[967 1410 130 100]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[270 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalibTof5000</t>
+  </si>
+  <si>
+    <t>[967 1410 130 100]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[270 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeBoBmTof5000</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>BMPDloopTof5000</t>
+  </si>
+  <si>
+    <t>[891 1407 180 85]</t>
+  </si>
+  <si>
+    <t>[2 1]</t>
+  </si>
+  <si>
+    <t>[700 100]</t>
+  </si>
+  <si>
+    <t>BMPDloopTof5000</t>
+  </si>
+  <si>
+    <t>[891 1407 180 100]</t>
+  </si>
+  <si>
+    <t>[2 1]</t>
+  </si>
+  <si>
+    <t>[750 100]</t>
+  </si>
+  <si>
+    <t>BMPDloopTof5000</t>
+  </si>
+  <si>
+    <t>[941 1405 180 100]</t>
+  </si>
+  <si>
+    <t>[2 1]</t>
+  </si>
+  <si>
+    <t>[750 100]</t>
+  </si>
+  <si>
+    <t>EvapDOdt1</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>HfBecFullTof</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>HfBecFullTof</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalibTof5000</t>
+  </si>
+  <si>
+    <t>[1024 1328 130 100]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[270 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeDepthCalibTof5000</t>
+  </si>
+  <si>
+    <t>[1024 1328 130 120]</t>
+  </si>
+  <si>
+    <t>[3 1]</t>
+  </si>
+  <si>
+    <t>[270 100]</t>
   </si>
 </sst>
 </file>
@@ -981,7 +1737,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -1042,19 +1798,19 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>197</v>
+        <v>437</v>
       </c>
       <c r="B2" s="0">
-        <v>450</v>
+        <v>334</v>
       </c>
       <c r="C2" s="0">
-        <v>1650</v>
+        <v>1668</v>
       </c>
       <c r="D2" s="0">
-        <v>700</v>
+        <v>530</v>
       </c>
       <c r="E2" s="0">
-        <v>1900</v>
+        <v>1970</v>
       </c>
       <c r="F2" s="0">
         <v>2160</v>
@@ -1066,13 +1822,13 @@
         <v>0</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>198</v>
+        <v>438</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>199</v>
+        <v>439</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>200</v>
+        <v>440</v>
       </c>
     </row>
     <row r="3">
@@ -1141,19 +1897,19 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>201</v>
+        <v>369</v>
       </c>
       <c r="B5" s="0">
-        <v>1121</v>
+        <v>911</v>
       </c>
       <c r="C5" s="0">
-        <v>1463</v>
+        <v>1183</v>
       </c>
       <c r="D5" s="0">
-        <v>1239</v>
+        <v>1235</v>
       </c>
       <c r="E5" s="0">
-        <v>1615</v>
+        <v>1511</v>
       </c>
       <c r="F5" s="0">
         <v>2160</v>
@@ -1162,16 +1918,16 @@
         <v>2560</v>
       </c>
       <c r="H5" s="0">
-        <v>349.10000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>202</v>
+        <v>370</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>203</v>
+        <v>371</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>204</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6">
@@ -1208,19 +1964,19 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>121</v>
+        <v>365</v>
       </c>
       <c r="B7" s="0">
-        <v>1060</v>
+        <v>778</v>
       </c>
       <c r="C7" s="0">
-        <v>1466</v>
+        <v>1372</v>
       </c>
       <c r="D7" s="0">
-        <v>1690</v>
+        <v>1286</v>
       </c>
       <c r="E7" s="0">
-        <v>1740</v>
+        <v>1442</v>
       </c>
       <c r="F7" s="0">
         <v>2160</v>
@@ -1229,33 +1985,33 @@
         <v>2560</v>
       </c>
       <c r="H7" s="0">
-        <v>349.10000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>122</v>
+        <v>366</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>123</v>
+        <v>367</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>124</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>133</v>
+        <v>377</v>
       </c>
       <c r="B8" s="0">
-        <v>1059</v>
+        <v>708</v>
       </c>
       <c r="C8" s="0">
-        <v>1467</v>
+        <v>1400</v>
       </c>
       <c r="D8" s="0">
-        <v>1684</v>
+        <v>1346</v>
       </c>
       <c r="E8" s="0">
-        <v>1756</v>
+        <v>1400</v>
       </c>
       <c r="F8" s="0">
         <v>2160</v>
@@ -1264,16 +2020,16 @@
         <v>2560</v>
       </c>
       <c r="H8" s="0">
-        <v>349.10000000000002</v>
+        <v>2.3000000000000003</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>134</v>
+        <v>378</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>135</v>
+        <v>379</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>136</v>
+        <v>380</v>
       </c>
     </row>
     <row r="9">
@@ -1453,19 +2209,19 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>185</v>
+        <v>385</v>
       </c>
       <c r="B14" s="0">
-        <v>1039</v>
+        <v>759</v>
       </c>
       <c r="C14" s="0">
-        <v>1499</v>
+        <v>1313</v>
       </c>
       <c r="D14" s="0">
-        <v>1631</v>
+        <v>1236</v>
       </c>
       <c r="E14" s="0">
-        <v>1765</v>
+        <v>1556</v>
       </c>
       <c r="F14" s="0">
         <v>2160</v>
@@ -1474,33 +2230,33 @@
         <v>2560</v>
       </c>
       <c r="H14" s="0">
-        <v>349.10000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>186</v>
+        <v>386</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>187</v>
+        <v>387</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>188</v>
+        <v>388</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>141</v>
+        <v>397</v>
       </c>
       <c r="B15" s="0">
-        <v>938</v>
+        <v>490</v>
       </c>
       <c r="C15" s="0">
-        <v>1666</v>
+        <v>1352</v>
       </c>
       <c r="D15" s="0">
-        <v>1619</v>
+        <v>1341</v>
       </c>
       <c r="E15" s="0">
-        <v>1773</v>
+        <v>1483</v>
       </c>
       <c r="F15" s="0">
         <v>2160</v>
@@ -1509,16 +2265,16 @@
         <v>2560</v>
       </c>
       <c r="H15" s="0">
-        <v>349.10000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>142</v>
+        <v>398</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>143</v>
+        <v>399</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>144</v>
+        <v>400</v>
       </c>
     </row>
     <row r="16">
@@ -1799,6 +2555,216 @@
       </c>
       <c r="K23" s="0" t="s">
         <v>196</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B24" s="0">
+        <v>510</v>
+      </c>
+      <c r="C24" s="0">
+        <v>1468</v>
+      </c>
+      <c r="D24" s="0">
+        <v>1333</v>
+      </c>
+      <c r="E24" s="0">
+        <v>1459</v>
+      </c>
+      <c r="F24" s="0">
+        <v>2160</v>
+      </c>
+      <c r="G24" s="0">
+        <v>2560</v>
+      </c>
+      <c r="H24" s="0">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="B25" s="0">
+        <v>454</v>
+      </c>
+      <c r="C25" s="0">
+        <v>1500</v>
+      </c>
+      <c r="D25" s="0">
+        <v>1365</v>
+      </c>
+      <c r="E25" s="0">
+        <v>1523</v>
+      </c>
+      <c r="F25" s="0">
+        <v>2160</v>
+      </c>
+      <c r="G25" s="0">
+        <v>2560</v>
+      </c>
+      <c r="H25" s="0">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="B26" s="0">
+        <v>634</v>
+      </c>
+      <c r="C26" s="0">
+        <v>1422</v>
+      </c>
+      <c r="D26" s="0">
+        <v>1333</v>
+      </c>
+      <c r="E26" s="0">
+        <v>1563</v>
+      </c>
+      <c r="F26" s="0">
+        <v>2160</v>
+      </c>
+      <c r="G26" s="0">
+        <v>2560</v>
+      </c>
+      <c r="H26" s="0">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="B27" s="0">
+        <v>709</v>
+      </c>
+      <c r="C27" s="0">
+        <v>1419</v>
+      </c>
+      <c r="D27" s="0">
+        <v>1287</v>
+      </c>
+      <c r="E27" s="0">
+        <v>1445</v>
+      </c>
+      <c r="F27" s="0">
+        <v>2160</v>
+      </c>
+      <c r="G27" s="0">
+        <v>2560</v>
+      </c>
+      <c r="H27" s="0">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="B28" s="0">
+        <v>582</v>
+      </c>
+      <c r="C28" s="0">
+        <v>1484</v>
+      </c>
+      <c r="D28" s="0">
+        <v>1385</v>
+      </c>
+      <c r="E28" s="0">
+        <v>1505</v>
+      </c>
+      <c r="F28" s="0">
+        <v>2160</v>
+      </c>
+      <c r="G28" s="0">
+        <v>2560</v>
+      </c>
+      <c r="H28" s="0">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="B29" s="0">
+        <v>736</v>
+      </c>
+      <c r="C29" s="0">
+        <v>1358</v>
+      </c>
+      <c r="D29" s="0">
+        <v>1060</v>
+      </c>
+      <c r="E29" s="0">
+        <v>1686</v>
+      </c>
+      <c r="F29" s="0">
+        <v>2160</v>
+      </c>
+      <c r="G29" s="0">
+        <v>2560</v>
+      </c>
+      <c r="H29" s="0">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="K29" s="0" t="s">
+        <v>448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated scope value plot
</commit_message>
<xml_diff>
--- a/.config/acquisitionConfig/roi.csv.xlsx
+++ b/.config/acquisitionConfig/roi.csv.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="473">
   <si>
     <t>Angle</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1411,6 +1411,54 @@
   </si>
   <si>
     <t>[270 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeBoBmTof5000</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>NiLatticeBoBmTof5000</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[1 1]</t>
+  </si>
+  <si>
+    <t>[100 100]</t>
+  </si>
+  <si>
+    <t>BMPDloopTof5000</t>
+  </si>
+  <si>
+    <t>[939 1345 180 100]</t>
+  </si>
+  <si>
+    <t>[2 1]</t>
+  </si>
+  <si>
+    <t>[750 100]</t>
+  </si>
+  <si>
+    <t>BMPDloopTof4000</t>
+  </si>
+  <si>
+    <t>[939 1345 180 100]</t>
+  </si>
+  <si>
+    <t>[2 1]</t>
+  </si>
+  <si>
+    <t>[600 100]</t>
   </si>
 </sst>
 </file>
@@ -1737,7 +1785,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -2594,19 +2642,19 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>433</v>
+        <v>465</v>
       </c>
       <c r="B25" s="0">
-        <v>454</v>
+        <v>487</v>
       </c>
       <c r="C25" s="0">
-        <v>1500</v>
+        <v>1545</v>
       </c>
       <c r="D25" s="0">
-        <v>1365</v>
+        <v>1299</v>
       </c>
       <c r="E25" s="0">
-        <v>1523</v>
+        <v>1473</v>
       </c>
       <c r="F25" s="0">
         <v>2160</v>
@@ -2618,13 +2666,13 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>434</v>
+        <v>466</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>435</v>
+        <v>467</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>436</v>
+        <v>468</v>
       </c>
     </row>
     <row r="26">
@@ -2699,19 +2747,19 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>421</v>
+        <v>461</v>
       </c>
       <c r="B28" s="0">
-        <v>582</v>
+        <v>648</v>
       </c>
       <c r="C28" s="0">
-        <v>1484</v>
+        <v>1374</v>
       </c>
       <c r="D28" s="0">
-        <v>1385</v>
+        <v>1297</v>
       </c>
       <c r="E28" s="0">
-        <v>1505</v>
+        <v>1443</v>
       </c>
       <c r="F28" s="0">
         <v>2160</v>
@@ -2723,13 +2771,13 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>422</v>
+        <v>462</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>423</v>
+        <v>463</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>424</v>
+        <v>464</v>
       </c>
     </row>
     <row r="29">
@@ -2765,6 +2813,41 @@
       </c>
       <c r="K29" s="0" t="s">
         <v>448</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="B30" s="0">
+        <v>487</v>
+      </c>
+      <c r="C30" s="0">
+        <v>1545</v>
+      </c>
+      <c r="D30" s="0">
+        <v>1299</v>
+      </c>
+      <c r="E30" s="0">
+        <v>1473</v>
+      </c>
+      <c r="F30" s="0">
+        <v>2160</v>
+      </c>
+      <c r="G30" s="0">
+        <v>2560</v>
+      </c>
+      <c r="H30" s="0">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="K30" s="0" t="s">
+        <v>472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>